<commit_message>
Added Page Object and WebDriverKeyowrds
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/hrm_data.xlsx
+++ b/src/test/resources/test_data/hrm_data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="validLoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="addEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +59,18 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>test fname</t>
+  </si>
+  <si>
+    <t>test lname</t>
   </si>
 </sst>
 </file>
@@ -426,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,4 +482,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>